<commit_message>
fixed authorship for alak1253-1
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-alak1253-1.xlsx
+++ b/raw/xlsx/numerals-alak1253-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865D5CE-1A63-7246-8733-D96D823EFA00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD13E977-72BE-D344-BE89-BA084590332C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="28280" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="28280" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -101,12 +101,6 @@
     <t>Alak.htm</t>
   </si>
   <si>
-    <t>Mr. Ryan Gehrmann, Graduate Student, Linguistics 
-Department, Payap University, Thailand, February 23, 2021. Sources: 
-    Luangthongkum, Theraphan. 2001. ภาษาของนานาชนเผ่าในแขวงเชกองลาวใต้. Phasa khong nana chon phaw nai khweng se kong lao tai. [Languages of the tribes in Xekong province southern Laos]. Bangkok: The Thailand Research Fund. 
-    Huffman, Franklin. 1971. Vocabulary lists for Loven, Souei and Alak. In Paul Sidwell (ed.), Huffman Papers. Online: huffman (Accessed 23 February, 2021).</t>
-  </si>
-  <si>
     <t>Gehrmann</t>
   </si>
   <si>
@@ -210,6 +204,9 @@
   </si>
   <si>
     <t>ban</t>
+  </si>
+  <si>
+    <t>Mr. Ryan Gehrmann, Graduate Student, Linguistics, Department, Payap University, Thailand, February 23, 2021. Sources: Luangthongkum, Theraphan. 2001. ภาษาของนานาชนเผ่าในแขวงเชกองลาวใต้. Phasa khong nana chon phaw nai khweng se kong lao tai. [Languages of the tribes in Xekong province southern Laos]. Bangkok: The Thailand Research Fund. Huffman, Franklin. 1971. Vocabulary lists for Loven, Souei and Alak. In Paul Sidwell (ed.), Huffman Papers. Online: huffman (Accessed 23 February, 2021).</t>
   </si>
 </sst>
 </file>
@@ -592,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
@@ -623,199 +620,199 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -830,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -885,15 +882,15 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -901,15 +898,15 @@
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="186" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="124" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -929,7 +926,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -946,12 +943,12 @@
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>